<commit_message>
updates to make it generalised
</commit_message>
<xml_diff>
--- a/data/Apple_AF_Steinfurt_wRisk_30.xlsx
+++ b/data/Apple_AF_Steinfurt_wRisk_30.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajna\Documents\HORTIBONN\PROJECTS\REFOREST\data\Apple_Agroforestry_System\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajna\Documents\HORTIBONN\PROJECTS\REFOREST\from_partners\EMEA\DA_model\AFDAtool_EMEA_Financial_Scheme\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3496591E-EC13-4077-8E3E-BEB4F6A6CA98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C87EA48-159F-4FC4-91A6-E2A5CEF8EED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="815" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet_names" sheetId="2" r:id="rId1"/>
@@ -22,13 +22,14 @@
     <sheet name="Sheet6" sheetId="10" r:id="rId7"/>
     <sheet name="Sheet7" sheetId="11" r:id="rId8"/>
     <sheet name="Sheet8" sheetId="12" r:id="rId9"/>
+    <sheet name="Sheet9" sheetId="15" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="318">
   <si>
     <t>variable</t>
   </si>
@@ -468,9 +469,6 @@
     <t>N years</t>
   </si>
   <si>
-    <t>Timescope [years]</t>
-  </si>
-  <si>
     <t>%</t>
   </si>
   <si>
@@ -483,9 +481,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>Model iterations</t>
-  </si>
-  <si>
     <t>Number of model simulation runs</t>
   </si>
   <si>
@@ -525,9 +520,6 @@
     <t>Probability of extreme weather</t>
   </si>
   <si>
-    <t>Agroforestry farming</t>
-  </si>
-  <si>
     <t>chance_extreme_weather_t</t>
   </si>
   <si>
@@ -537,105 +529,6 @@
     <t>Absolute increment in tree yield</t>
   </si>
   <si>
-    <t>Wheat Yield coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Wheat Value coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Wheat Seed Price coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Wheat Insurance coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Maize Yield coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Maize Value coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Maize Seed Price coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Maize Insurance coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Barley Yield coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Barley Value coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Barley Seed Price coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Barley Insurance coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Rapeseed Yield coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Wheat Fertilizer Price coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Wheat Pesticides Price coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Wheat Machinery Price coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Wheat Labour Price coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Maize Fertilizer Price coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Maize Pesticides Price coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Maize Machinery Price coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Maize Labour Price coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Barley Fertilizer Price coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Barley Pesticides Price coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Barley Machinery Price coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Barley Labour Price coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Rapeseed Value coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Rapeseed Seed Price coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Rapeseed Fertilizer Price coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Rapeseed Pesticides Price coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Rapeseed Machinery Price coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Rapeseed Labour Price coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Rapeseed Insurance coefficient of variation [%]</t>
-  </si>
-  <si>
-    <t>Maximum Reduction possible due to trees</t>
-  </si>
-  <si>
     <t>Risk that irrigation system needs repair</t>
   </si>
   <si>
@@ -645,78 +538,21 @@
     <t>€</t>
   </si>
   <si>
-    <t xml:space="preserve">Cost of pruning course for employee </t>
-  </si>
-  <si>
     <t>Water use in frist three years of tree establishment</t>
   </si>
   <si>
     <t>Water use in annual irrigation</t>
   </si>
   <si>
-    <t>Labour hours for pruning juvenile apple trees (year 1-5)</t>
-  </si>
-  <si>
-    <t>Labour hours for pruning juvenile apple trees (6-10)</t>
-  </si>
-  <si>
-    <t>Labour hours for pruning mature apple trees (year 11-15)</t>
-  </si>
-  <si>
-    <t>Labour hours for pruning mature apple trees (year 16 onwards)</t>
-  </si>
-  <si>
     <t>Labour hours for root pruning trees</t>
   </si>
   <si>
     <t>Labour hours for mowing the tree strips manually</t>
   </si>
   <si>
-    <t>Price of table apples</t>
-  </si>
-  <si>
-    <t>Price of intermediate quality apples</t>
-  </si>
-  <si>
     <t>€/kg</t>
   </si>
   <si>
-    <t xml:space="preserve">Price of juice apples </t>
-  </si>
-  <si>
-    <t>First apple yield, % of max. apple yield</t>
-  </si>
-  <si>
-    <t>Second stage apple yield, % of max. apple yield</t>
-  </si>
-  <si>
-    <t>Maximum apple yield</t>
-  </si>
-  <si>
-    <t>Estimate 1 when apple trees produce first harvest</t>
-  </si>
-  <si>
-    <t>Estimate 2 when apple trees produce first harvest</t>
-  </si>
-  <si>
-    <t>Estimate 1 when apple trees reach second yield stage (for gompertz curve)</t>
-  </si>
-  <si>
-    <t>Estimate 2 when apple trees reach second yield stage (for gompertz curve)</t>
-  </si>
-  <si>
-    <t>Labour cost for harvesting a kg of apples</t>
-  </si>
-  <si>
-    <t>Post Harvest loss of Apple</t>
-  </si>
-  <si>
-    <t>Percentage of total apple yield with table apple quality</t>
-  </si>
-  <si>
-    <t>Percentage of intermediate quality apples</t>
-  </si>
-  <si>
     <t>Time spent discussing goals with consultants, planning AF system and other planning work done by farmer</t>
   </si>
   <si>
@@ -756,9 +592,6 @@
     <t>Labour hours of planting tree</t>
   </si>
   <si>
-    <t>Price per apple tree (tree only)</t>
-  </si>
-  <si>
     <t>Cost of mesh for protection against vole damage</t>
   </si>
   <si>
@@ -789,45 +622,15 @@
     <t>Total area of tree rows (wooded area) in AF system</t>
   </si>
   <si>
-    <t>Number of apple trees planted in AF system</t>
-  </si>
-  <si>
     <t>ha</t>
   </si>
   <si>
     <t>Labour hours for measuring field with GPS, identifying placement of trees</t>
   </si>
   <si>
-    <t>Estimate 1 when reduced produce first harvest of crop</t>
-  </si>
-  <si>
-    <t>Estimate 2 when reduced produce second harvest of crop</t>
-  </si>
-  <si>
-    <t>Percentage max first reduction</t>
-  </si>
-  <si>
-    <t>Percentage max second reduction</t>
-  </si>
-  <si>
-    <t>Agroforestry farming;Data analyst</t>
-  </si>
-  <si>
     <t>t/ha</t>
   </si>
   <si>
-    <t>Maize yield [t/ha]</t>
-  </si>
-  <si>
-    <t>Wheat yield [t/ha]</t>
-  </si>
-  <si>
-    <t>Barley yield [t/ha]</t>
-  </si>
-  <si>
-    <t>Rapeseed yield [t/ha]</t>
-  </si>
-  <si>
     <t>€/ha</t>
   </si>
   <si>
@@ -837,93 +640,24 @@
     <t>€/t</t>
   </si>
   <si>
-    <t>Cost of Maize seed [€/ha]</t>
-  </si>
-  <si>
-    <t>Cost of Rapeseed seed [€/ha]</t>
-  </si>
-  <si>
-    <t>Value of maize [€/t]</t>
-  </si>
-  <si>
     <t>Cost of fertilizer (NPK + Lime)  [€/ha]</t>
   </si>
   <si>
-    <t>Cost of pesticides used in conventional maize field  [€/ha]</t>
-  </si>
-  <si>
-    <t>Machine cost for Maize management, fixed and variable machine cost  [€/ha]</t>
-  </si>
-  <si>
     <t>Labour hours for Maize management  [h/ha]</t>
   </si>
   <si>
-    <t>Cost of Maize insurance  [€/ha]</t>
-  </si>
-  <si>
-    <t>Cost of Wheat insurance  [€/ha]</t>
-  </si>
-  <si>
-    <t>Cost of Rapeseed insurance  [€/ha]</t>
-  </si>
-  <si>
-    <t>Cost of Barley seed [€/ha]</t>
-  </si>
-  <si>
-    <t>Value of Barley [€/t]</t>
-  </si>
-  <si>
-    <t>Cost of fertilizer for Barley (NPK + Lime)  [€/ha]</t>
-  </si>
-  <si>
-    <t>Cost of pesticides used in conventional Barley field  [€/ha]</t>
-  </si>
-  <si>
-    <t>Machine cost for Barley management, fixed and variable machine cost  [€/ha]</t>
-  </si>
-  <si>
     <t>Labour hours for Barley management  [h/ha]</t>
   </si>
   <si>
-    <t>Cost of Barley insurance  [€/ha]</t>
-  </si>
-  <si>
-    <t>Value of Rapeseed [€/t]</t>
-  </si>
-  <si>
-    <t>Cost of fertilizer for Rapeseed (NPK + Lime)  [€/ha]</t>
-  </si>
-  <si>
-    <t>Cost of pesticides used in conventional Rapeseed field  [€/ha]</t>
-  </si>
-  <si>
-    <t>Machine cost for Rapeseed management, fixed and variable machine cost  [€/ha]</t>
-  </si>
-  <si>
     <t>Labour hours for Rapeseed management  [h/ha]</t>
   </si>
   <si>
-    <t>Value of Wheat [€/t]</t>
-  </si>
-  <si>
-    <t>Cost of fertilizer for Wheat (NPK + Lime)  [€/ha]</t>
-  </si>
-  <si>
-    <t>Cost of pesticides used in conventional Wheat field  [€/ha]</t>
-  </si>
-  <si>
-    <t>Machine cost for Wheat management, fixed and variable machine cost  [€/ha]</t>
-  </si>
-  <si>
     <t>Labour hours for Wheat management  [h/ha]</t>
   </si>
   <si>
     <t>Size of the arable field [ha]</t>
   </si>
   <si>
-    <t>Data analyst; Agroforestry farming</t>
-  </si>
-  <si>
     <t>Risks</t>
   </si>
   <si>
@@ -939,9 +673,6 @@
     <t>Annual maintenance support: Lump sum of funds received annually from external sources in order to maintain the agroforestry system [€]</t>
   </si>
   <si>
-    <t>Policy analysis;Agroforestry farming</t>
-  </si>
-  <si>
     <t>selected_percentage_c</t>
   </si>
   <si>
@@ -973,6 +704,352 @@
   </si>
   <si>
     <t>Establishment funding support: Lump sum of funds received only once from external sources, regardless of the investment costs [€]</t>
+  </si>
+  <si>
+    <t>Simulation period [years]</t>
+  </si>
+  <si>
+    <t>Number of model iterations</t>
+  </si>
+  <si>
+    <t>Number of trees planted in AF system</t>
+  </si>
+  <si>
+    <t>Price per tree (tree only!)</t>
+  </si>
+  <si>
+    <t>Crop 1 yield [t/ha]</t>
+  </si>
+  <si>
+    <t>Machine cost for Crop 1 management, fixed and variable machine cost  [€/ha]</t>
+  </si>
+  <si>
+    <t>Cost of Crop 1 insurance  [€/ha]</t>
+  </si>
+  <si>
+    <t>Cost of Crop 1 seed [€/ha]</t>
+  </si>
+  <si>
+    <t>Value of Crop 1 [€/t]</t>
+  </si>
+  <si>
+    <t>Cost of pesticides used in conventional Crop 1 field  [€/ha]</t>
+  </si>
+  <si>
+    <t>Value of Crop 2 [€/t]</t>
+  </si>
+  <si>
+    <t>Cost of fertilizer for Crop 2 (NPK + Lime)  [€/ha]</t>
+  </si>
+  <si>
+    <t>Cost of pesticides used in conventional Crop 2 field  [€/ha]</t>
+  </si>
+  <si>
+    <t>Machine cost for Crop 2 management, fixed and variable machine cost  [€/ha]</t>
+  </si>
+  <si>
+    <t>Cost of Crop 2 insurance  [€/ha]</t>
+  </si>
+  <si>
+    <t>Crop 2 yield [t/ha]</t>
+  </si>
+  <si>
+    <t>Crop 3 yield [t/ha]</t>
+  </si>
+  <si>
+    <t>Cost of Crop 3 seed [€/ha]</t>
+  </si>
+  <si>
+    <t>Value of Crop 3 [€/t]</t>
+  </si>
+  <si>
+    <t>Cost of fertilizer for Crop 3 (NPK + Lime)  [€/ha]</t>
+  </si>
+  <si>
+    <t>Cost of pesticides used in conventional Crop 3 field  [€/ha]</t>
+  </si>
+  <si>
+    <t>Machine cost for Crop 3 management, fixed and variable machine cost  [€/ha]</t>
+  </si>
+  <si>
+    <t>Cost of Crop 3 insurance  [€/ha]</t>
+  </si>
+  <si>
+    <t>Crop 4 yield [t/ha]</t>
+  </si>
+  <si>
+    <t>Cost of Crop 4 seed [€/ha]</t>
+  </si>
+  <si>
+    <t>Value of Crop 4 [€/t]</t>
+  </si>
+  <si>
+    <t>Cost of fertilizer for Crop 4 (NPK + Lime)  [€/ha]</t>
+  </si>
+  <si>
+    <t>Cost of pesticides used in conventional Crop 4 field  [€/ha]</t>
+  </si>
+  <si>
+    <t>Machine cost for Crop 4 management, fixed and variable machine cost  [€/ha]</t>
+  </si>
+  <si>
+    <t>Cost of Crop 4 insurance  [€/ha]</t>
+  </si>
+  <si>
+    <t>Data analyst;Farmer;Policy-maker;Market analyst;Investors;Advisors</t>
+  </si>
+  <si>
+    <t>Labour hours for pruning juvenile trees (year 1-5)</t>
+  </si>
+  <si>
+    <t>Labour hours for pruning juvenile trees (6-10)</t>
+  </si>
+  <si>
+    <t>Labour hours for pruning mature trees (year 11-15)</t>
+  </si>
+  <si>
+    <t>Labour hours for pruning mature trees (year 16 onwards)</t>
+  </si>
+  <si>
+    <t>Maximum tree yield (fruits, nuts etc.)</t>
+  </si>
+  <si>
+    <t>Labour cost for harvesting a kg of tree yield</t>
+  </si>
+  <si>
+    <t>Post Harvest loss of tree yield</t>
+  </si>
+  <si>
+    <t>Price of 'A' grade tree yield (fruits, nuts etc.)</t>
+  </si>
+  <si>
+    <t>Price of 'B' grade tree yield (fruits, nuts etc.)</t>
+  </si>
+  <si>
+    <t>Price of 'C' grade tree (fruits, nuts etc.)</t>
+  </si>
+  <si>
+    <t>Percentage of 'A' grade tree yield of the total tree yield</t>
+  </si>
+  <si>
+    <t>Maximum possible reduction in crop yield due to trees</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Year in which arable crops reach their </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>first reduced yield level</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>due to shading or competition from trees</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Percentage maximum yield arable crop produce in that year (first reduced yield level )</t>
+  </si>
+  <si>
+    <t>Percentage maximum yield arable crop produce in that year (second rediced yield level)</t>
+  </si>
+  <si>
+    <t>Cost of pruning course for employees [€]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Year in which arable crops reach their </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>second reduced yield level</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (due to shading or competition from trees)</t>
+    </r>
+  </si>
+  <si>
+    <t>Soonest year of first harvest expected from your trees (fruits, nuts, etc.)- for Gompertz curve)</t>
+  </si>
+  <si>
+    <t>Latest year of first harvest expected from your trees (fruits, nuts, etc.)- for Gompertz curve)</t>
+  </si>
+  <si>
+    <t>Soonest year of second harvest expected from your trees (fruits, nuts, etc.)- for Gompertz curve)</t>
+  </si>
+  <si>
+    <t>Latest year of second harvest expected from your trees (fruits, nuts, etc.)- for Gompertz curve)</t>
+  </si>
+  <si>
+    <t>Percentage maximum yield tree yield produced in that year (second yield level )</t>
+  </si>
+  <si>
+    <t>Percentage maximum yield tree yield produced in that year (first yield level )</t>
+  </si>
+  <si>
+    <t>Crop 4 Yield coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 4 Value coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 4 Seed Price coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 4 Fertilizer Price coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 4 Pesticides Price coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 4 Machinery Price coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 4 Labour Price coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 4 Insurance coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 1 Yield coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 1 Value coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 1 Seed Price coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 1 Fertilizer Price coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 1 Pesticides Price coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 1 Machinery Price coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 1 Labour Price coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 1 Insurance coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 2 Yield coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 2 Value coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 2 Seed Price coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 2 Fertilizer Price coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 2 Pesticides Price coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 2 Machinery Price coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 2 Labour Price coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 2 Insurance coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 3 Yield coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 3 Value coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 3 Seed Price coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 3 Fertilizer Price coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 3 Pesticides Price coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 3 Machinery Price coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 3 Labour Price coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Crop 3 Insurance coefficient of variation [%]</t>
+  </si>
+  <si>
+    <t>Data analyst;Farmer;Policy-maker;Advisors</t>
+  </si>
+  <si>
+    <t>Data analyst;Farmer</t>
+  </si>
+  <si>
+    <t>Data analyst;Farmer;Policy-maker;Investors;Advisors</t>
+  </si>
+  <si>
+    <t>Data analyst;Farmer;Investors;Advisors</t>
+  </si>
+  <si>
+    <t>Data analyst;Farmer;Advisors</t>
+  </si>
+  <si>
+    <t>EMEA's Financial Scheme</t>
+  </si>
+  <si>
+    <t>coins</t>
   </si>
 </sst>
 </file>
@@ -982,7 +1059,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -997,6 +1074,22 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1322,10 +1415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19247B9C-F4A5-4DCC-BF21-E18D3CC8C8F5}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1384,7 +1477,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>298</v>
+        <v>209</v>
       </c>
       <c r="B7" t="s">
         <v>142</v>
@@ -1392,7 +1485,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>299</v>
+        <v>210</v>
       </c>
       <c r="B8" t="s">
         <v>139</v>
@@ -1404,6 +1497,64 @@
       </c>
       <c r="B9" t="s">
         <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>316</v>
+      </c>
+      <c r="B10" t="s">
+        <v>317</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C0A4C84-585F-4989-ACDA-A26FA8E30FDB}">
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P29" sqref="P29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" t="s">
+        <v>155</v>
+      </c>
+      <c r="J1" t="s">
+        <v>156</v>
+      </c>
+      <c r="K1" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1422,6 +1573,8 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" customWidth="1"/>
+    <col min="10" max="10" width="29.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -1444,19 +1597,19 @@
         <v>144</v>
       </c>
       <c r="G1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" t="s">
         <v>155</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>156</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>157</v>
-      </c>
-      <c r="J1" t="s">
-        <v>158</v>
-      </c>
-      <c r="K1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1476,16 +1629,16 @@
         <v>145</v>
       </c>
       <c r="F2" t="s">
-        <v>146</v>
+        <v>225</v>
       </c>
       <c r="H2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I2">
         <v>1000</v>
       </c>
       <c r="J2" t="s">
-        <v>165</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1502,22 +1655,22 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>297</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1534,19 +1687,19 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F4" t="s">
         <v>147</v>
       </c>
-      <c r="F4" t="s">
-        <v>148</v>
-      </c>
       <c r="H4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>154</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -1563,24 +1716,24 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>254</v>
+        <v>197</v>
       </c>
       <c r="F5" t="s">
-        <v>296</v>
+        <v>208</v>
       </c>
       <c r="H5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I5">
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>154</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B6" s="1">
         <v>1000</v>
@@ -1592,22 +1745,22 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F6" t="s">
+        <v>226</v>
+      </c>
+      <c r="G6" t="s">
         <v>150</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>151</v>
       </c>
-      <c r="G6" t="s">
-        <v>152</v>
-      </c>
-      <c r="H6" t="s">
-        <v>153</v>
-      </c>
       <c r="I6">
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>154</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -1620,12 +1773,14 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="J2" sqref="J2:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -1648,19 +1803,19 @@
         <v>144</v>
       </c>
       <c r="G1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" t="s">
         <v>155</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>156</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>157</v>
-      </c>
-      <c r="J1" t="s">
-        <v>158</v>
-      </c>
-      <c r="K1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1677,19 +1832,19 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>254</v>
+        <v>197</v>
       </c>
       <c r="F2" t="s">
-        <v>252</v>
+        <v>196</v>
       </c>
       <c r="H2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I2">
         <v>0.1</v>
       </c>
       <c r="J2" t="s">
-        <v>165</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1706,16 +1861,16 @@
         <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>253</v>
+        <v>227</v>
       </c>
       <c r="H3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I3">
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>165</v>
+        <v>311</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1732,219 +1887,219 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>255</v>
+        <v>198</v>
       </c>
       <c r="H4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>165</v>
+        <v>311</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B5">
-        <v>5.0000000000000004E-6</v>
+        <v>0.09</v>
       </c>
       <c r="C5">
-        <v>3.1E-4</v>
+        <v>0.13</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>238</v>
+        <v>185</v>
       </c>
       <c r="F5" t="s">
-        <v>237</v>
+        <v>184</v>
       </c>
       <c r="H5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I5">
-        <v>9.9999999999999995E-7</v>
+        <v>0.01</v>
       </c>
       <c r="J5" t="s">
-        <v>165</v>
+        <v>311</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6">
-        <v>0.09</v>
+        <v>0.5</v>
       </c>
       <c r="C6">
-        <v>0.13</v>
+        <v>1.5</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>240</v>
+        <v>185</v>
       </c>
       <c r="F6" t="s">
-        <v>239</v>
+        <v>186</v>
       </c>
       <c r="H6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I6">
         <v>0.01</v>
       </c>
       <c r="J6" t="s">
-        <v>165</v>
+        <v>311</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7">
-        <v>0.5</v>
+        <v>10</v>
       </c>
       <c r="C7">
-        <v>1.5</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>240</v>
+        <v>185</v>
       </c>
       <c r="F7" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="H7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I7">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>165</v>
+        <v>311</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>9.0500000000000007</v>
       </c>
       <c r="C8">
-        <v>20</v>
+        <v>11.75</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>240</v>
+        <v>185</v>
       </c>
       <c r="F8" t="s">
-        <v>242</v>
+        <v>187</v>
       </c>
       <c r="H8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I8">
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>165</v>
+        <v>311</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B9">
-        <v>9.0500000000000007</v>
+        <v>1.18</v>
       </c>
       <c r="C9">
-        <v>11.75</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>240</v>
+        <v>185</v>
       </c>
       <c r="F9" t="s">
-        <v>243</v>
+        <v>188</v>
       </c>
       <c r="H9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>165</v>
+        <v>311</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10">
-        <v>1.18</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>1.6</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>240</v>
+        <v>185</v>
       </c>
       <c r="F10" t="s">
-        <v>244</v>
+        <v>189</v>
       </c>
       <c r="H10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="J10" t="s">
-        <v>165</v>
+        <v>311</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>1.1499999999999999</v>
+        <v>5.0000000000000004E-6</v>
       </c>
       <c r="C11">
-        <v>1.6</v>
+        <v>3.1E-4</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>240</v>
+        <v>183</v>
       </c>
       <c r="F11" t="s">
-        <v>245</v>
+        <v>182</v>
       </c>
       <c r="H11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I11">
-        <v>0.1</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="J11" t="s">
-        <v>165</v>
+        <v>311</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1961,19 +2116,19 @@
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>204</v>
+        <v>168</v>
       </c>
       <c r="F12" t="s">
-        <v>246</v>
+        <v>190</v>
       </c>
       <c r="H12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I12">
         <v>100</v>
       </c>
       <c r="J12" t="s">
-        <v>165</v>
+        <v>311</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1990,19 +2145,19 @@
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>248</v>
+        <v>192</v>
       </c>
       <c r="F13" t="s">
-        <v>247</v>
+        <v>191</v>
       </c>
       <c r="H13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I13">
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>165</v>
+        <v>311</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -2019,19 +2174,19 @@
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>248</v>
+        <v>192</v>
       </c>
       <c r="F14" t="s">
-        <v>249</v>
+        <v>193</v>
       </c>
       <c r="H14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I14">
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>165</v>
+        <v>311</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -2048,19 +2203,19 @@
         <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>238</v>
+        <v>183</v>
       </c>
       <c r="F15" t="s">
-        <v>250</v>
+        <v>194</v>
       </c>
       <c r="H15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I15">
         <v>0.1</v>
       </c>
       <c r="J15" t="s">
-        <v>165</v>
+        <v>311</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -2077,19 +2232,19 @@
         <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>248</v>
+        <v>192</v>
       </c>
       <c r="F16" t="s">
-        <v>251</v>
+        <v>195</v>
       </c>
       <c r="H16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I16">
         <v>10</v>
       </c>
       <c r="J16" t="s">
-        <v>165</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -2102,7 +2257,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="J2" sqref="J2:J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2131,19 +2286,19 @@
         <v>144</v>
       </c>
       <c r="G1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" t="s">
         <v>155</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>156</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>157</v>
-      </c>
-      <c r="J1" t="s">
-        <v>158</v>
-      </c>
-      <c r="K1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -2160,19 +2315,19 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>261</v>
+        <v>199</v>
       </c>
       <c r="F2" t="s">
-        <v>262</v>
+        <v>229</v>
       </c>
       <c r="H2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>165</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -2189,19 +2344,19 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>261</v>
+        <v>199</v>
       </c>
       <c r="F3" t="s">
-        <v>263</v>
+        <v>240</v>
       </c>
       <c r="H3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>165</v>
+        <v>312</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -2218,19 +2373,19 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>261</v>
+        <v>199</v>
       </c>
       <c r="F4" t="s">
-        <v>264</v>
+        <v>241</v>
       </c>
       <c r="H4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>165</v>
+        <v>312</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -2247,19 +2402,19 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>261</v>
+        <v>199</v>
       </c>
       <c r="F5" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
       <c r="H5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I5">
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>165</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -2276,19 +2431,19 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>266</v>
+        <v>200</v>
       </c>
       <c r="F6" t="s">
-        <v>269</v>
+        <v>232</v>
       </c>
       <c r="H6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I6">
         <v>10</v>
       </c>
       <c r="J6" t="s">
-        <v>165</v>
+        <v>312</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -2305,19 +2460,19 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>268</v>
+        <v>202</v>
       </c>
       <c r="F7" t="s">
-        <v>271</v>
+        <v>233</v>
       </c>
       <c r="H7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I7">
         <v>10</v>
       </c>
       <c r="J7" t="s">
-        <v>165</v>
+        <v>312</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -2334,19 +2489,19 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>266</v>
+        <v>200</v>
       </c>
       <c r="F8" t="s">
-        <v>272</v>
+        <v>203</v>
       </c>
       <c r="H8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I8">
         <v>10</v>
       </c>
       <c r="J8" t="s">
-        <v>165</v>
+        <v>312</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -2363,19 +2518,19 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>266</v>
+        <v>200</v>
       </c>
       <c r="F9" t="s">
-        <v>273</v>
+        <v>234</v>
       </c>
       <c r="H9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I9">
         <v>10</v>
       </c>
       <c r="J9" t="s">
-        <v>165</v>
+        <v>312</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -2392,19 +2547,19 @@
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>266</v>
+        <v>200</v>
       </c>
       <c r="F10" t="s">
-        <v>274</v>
+        <v>230</v>
       </c>
       <c r="H10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I10">
         <v>10</v>
       </c>
       <c r="J10" t="s">
-        <v>165</v>
+        <v>312</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -2421,19 +2576,19 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>266</v>
+        <v>200</v>
       </c>
       <c r="F11" t="s">
-        <v>276</v>
+        <v>231</v>
       </c>
       <c r="H11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I11">
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>165</v>
+        <v>312</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -2450,19 +2605,19 @@
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>266</v>
+        <v>200</v>
       </c>
       <c r="F12" t="s">
-        <v>269</v>
+        <v>232</v>
       </c>
       <c r="H12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I12">
         <v>10</v>
       </c>
       <c r="J12" t="s">
-        <v>165</v>
+        <v>312</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -2479,19 +2634,19 @@
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>268</v>
+        <v>202</v>
       </c>
       <c r="F13" t="s">
-        <v>291</v>
+        <v>235</v>
       </c>
       <c r="H13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I13">
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>165</v>
+        <v>312</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -2508,19 +2663,19 @@
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>266</v>
+        <v>200</v>
       </c>
       <c r="F14" t="s">
-        <v>292</v>
+        <v>236</v>
       </c>
       <c r="H14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I14">
         <v>10</v>
       </c>
       <c r="J14" t="s">
-        <v>165</v>
+        <v>312</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -2537,19 +2692,19 @@
         <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>266</v>
+        <v>200</v>
       </c>
       <c r="F15" t="s">
-        <v>293</v>
+        <v>237</v>
       </c>
       <c r="H15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I15">
         <v>10</v>
       </c>
       <c r="J15" t="s">
-        <v>165</v>
+        <v>312</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -2566,19 +2721,19 @@
         <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>266</v>
+        <v>200</v>
       </c>
       <c r="F16" t="s">
-        <v>294</v>
+        <v>238</v>
       </c>
       <c r="H16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I16">
         <v>10</v>
       </c>
       <c r="J16" t="s">
-        <v>165</v>
+        <v>312</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -2595,19 +2750,19 @@
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>266</v>
+        <v>200</v>
       </c>
       <c r="F17" t="s">
-        <v>277</v>
+        <v>239</v>
       </c>
       <c r="H17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I17">
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>165</v>
+        <v>312</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -2624,19 +2779,19 @@
         <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>266</v>
+        <v>200</v>
       </c>
       <c r="F18" t="s">
-        <v>270</v>
+        <v>249</v>
       </c>
       <c r="H18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I18">
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>165</v>
+        <v>312</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -2653,19 +2808,19 @@
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>268</v>
+        <v>202</v>
       </c>
       <c r="F19" t="s">
-        <v>286</v>
+        <v>250</v>
       </c>
       <c r="H19" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I19">
         <v>10</v>
       </c>
       <c r="J19" t="s">
-        <v>165</v>
+        <v>312</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -2682,19 +2837,19 @@
         <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>266</v>
+        <v>200</v>
       </c>
       <c r="F20" t="s">
-        <v>287</v>
+        <v>251</v>
       </c>
       <c r="H20" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I20">
         <v>10</v>
       </c>
       <c r="J20" t="s">
-        <v>165</v>
+        <v>312</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -2711,19 +2866,19 @@
         <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>266</v>
+        <v>200</v>
       </c>
       <c r="F21" t="s">
-        <v>288</v>
+        <v>252</v>
       </c>
       <c r="H21" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I21">
         <v>10</v>
       </c>
       <c r="J21" t="s">
-        <v>165</v>
+        <v>312</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -2740,19 +2895,19 @@
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>266</v>
+        <v>200</v>
       </c>
       <c r="F22" t="s">
-        <v>289</v>
+        <v>253</v>
       </c>
       <c r="H22" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I22">
         <v>10</v>
       </c>
       <c r="J22" t="s">
-        <v>165</v>
+        <v>312</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -2769,19 +2924,19 @@
         <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>266</v>
+        <v>200</v>
       </c>
       <c r="F23" t="s">
-        <v>278</v>
+        <v>254</v>
       </c>
       <c r="H23" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I23">
         <v>5</v>
       </c>
       <c r="J23" t="s">
-        <v>165</v>
+        <v>312</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -2798,19 +2953,19 @@
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>266</v>
+        <v>200</v>
       </c>
       <c r="F24" t="s">
-        <v>279</v>
+        <v>242</v>
       </c>
       <c r="H24" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I24">
         <v>10</v>
       </c>
       <c r="J24" t="s">
-        <v>165</v>
+        <v>312</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -2827,19 +2982,19 @@
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>268</v>
+        <v>202</v>
       </c>
       <c r="F25" t="s">
-        <v>280</v>
+        <v>243</v>
       </c>
       <c r="H25" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I25">
         <v>10</v>
       </c>
       <c r="J25" t="s">
-        <v>165</v>
+        <v>312</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -2856,19 +3011,19 @@
         <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>266</v>
+        <v>200</v>
       </c>
       <c r="F26" t="s">
-        <v>281</v>
+        <v>244</v>
       </c>
       <c r="H26" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I26">
         <v>10</v>
       </c>
       <c r="J26" t="s">
-        <v>165</v>
+        <v>312</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -2885,19 +3040,19 @@
         <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>266</v>
+        <v>200</v>
       </c>
       <c r="F27" t="s">
-        <v>282</v>
+        <v>245</v>
       </c>
       <c r="H27" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I27">
         <v>10</v>
       </c>
       <c r="J27" t="s">
-        <v>165</v>
+        <v>312</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -2914,19 +3069,19 @@
         <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>266</v>
+        <v>200</v>
       </c>
       <c r="F28" t="s">
-        <v>283</v>
+        <v>246</v>
       </c>
       <c r="H28" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I28">
         <v>10</v>
       </c>
       <c r="J28" t="s">
-        <v>165</v>
+        <v>312</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -2943,19 +3098,19 @@
         <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>266</v>
+        <v>200</v>
       </c>
       <c r="F29" t="s">
-        <v>285</v>
+        <v>247</v>
       </c>
       <c r="H29" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I29">
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>165</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -2968,7 +3123,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2996,19 +3151,19 @@
         <v>144</v>
       </c>
       <c r="G1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" t="s">
         <v>155</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>156</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>157</v>
-      </c>
-      <c r="J1" t="s">
-        <v>158</v>
-      </c>
-      <c r="K1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -3025,19 +3180,19 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>230</v>
+        <v>175</v>
       </c>
       <c r="F2" t="s">
-        <v>229</v>
+        <v>174</v>
       </c>
       <c r="H2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I2">
         <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>260</v>
+        <v>313</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -3054,19 +3209,19 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>204</v>
+        <v>168</v>
       </c>
       <c r="F3" t="s">
-        <v>231</v>
+        <v>176</v>
       </c>
       <c r="H3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I3">
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>260</v>
+        <v>313</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -3083,19 +3238,19 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>233</v>
+        <v>178</v>
       </c>
       <c r="F4" t="s">
-        <v>232</v>
+        <v>177</v>
       </c>
       <c r="H4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I4">
         <v>5</v>
       </c>
       <c r="J4" t="s">
-        <v>260</v>
+        <v>313</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -3112,19 +3267,19 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>230</v>
+        <v>175</v>
       </c>
       <c r="F5" t="s">
-        <v>235</v>
+        <v>180</v>
       </c>
       <c r="H5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I5">
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>260</v>
+        <v>313</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -3141,19 +3296,19 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>230</v>
+        <v>175</v>
       </c>
       <c r="F6" t="s">
-        <v>234</v>
+        <v>179</v>
       </c>
       <c r="H6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I6">
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>260</v>
+        <v>313</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -3170,19 +3325,19 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F7" t="s">
-        <v>236</v>
+        <v>181</v>
       </c>
       <c r="H7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I7">
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>260</v>
+        <v>313</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -3199,19 +3354,19 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>267</v>
+        <v>201</v>
       </c>
       <c r="F8" t="s">
-        <v>284</v>
+        <v>205</v>
       </c>
       <c r="H8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I8">
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>260</v>
+        <v>313</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -3228,19 +3383,19 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>267</v>
+        <v>201</v>
       </c>
       <c r="F9" t="s">
-        <v>295</v>
+        <v>207</v>
       </c>
       <c r="H9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>260</v>
+        <v>313</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -3257,19 +3412,19 @@
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>267</v>
+        <v>201</v>
       </c>
       <c r="F10" t="s">
-        <v>290</v>
+        <v>206</v>
       </c>
       <c r="H10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>260</v>
+        <v>313</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -3286,19 +3441,19 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>267</v>
+        <v>201</v>
       </c>
       <c r="F11" t="s">
-        <v>275</v>
+        <v>204</v>
       </c>
       <c r="H11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I11">
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>260</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -3311,13 +3466,14 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" customWidth="1"/>
+    <col min="6" max="6" width="62.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -3340,19 +3496,19 @@
         <v>144</v>
       </c>
       <c r="G1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" t="s">
         <v>155</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>156</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>157</v>
-      </c>
-      <c r="J1" t="s">
-        <v>158</v>
-      </c>
-      <c r="K1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -3369,16 +3525,16 @@
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>205</v>
+        <v>271</v>
       </c>
       <c r="H2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I2">
         <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>165</v>
+        <v>314</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -3395,16 +3551,16 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>206</v>
+        <v>169</v>
       </c>
       <c r="H3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I3">
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>165</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -3421,16 +3577,16 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>207</v>
+        <v>170</v>
       </c>
       <c r="H4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I4">
         <v>5</v>
       </c>
       <c r="J4" t="s">
-        <v>165</v>
+        <v>314</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -3447,16 +3603,16 @@
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>208</v>
+        <v>256</v>
       </c>
       <c r="H5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I5">
         <v>0.01</v>
       </c>
       <c r="J5" t="s">
-        <v>165</v>
+        <v>314</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -3473,16 +3629,16 @@
         <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>209</v>
+        <v>257</v>
       </c>
       <c r="H6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I6">
         <v>0.01</v>
       </c>
       <c r="J6" t="s">
-        <v>165</v>
+        <v>314</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -3499,16 +3655,16 @@
         <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>210</v>
+        <v>258</v>
       </c>
       <c r="H7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I7">
         <v>0.1</v>
       </c>
       <c r="J7" t="s">
-        <v>165</v>
+        <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -3525,16 +3681,16 @@
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>211</v>
+        <v>259</v>
       </c>
       <c r="H8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I8">
         <v>0.01</v>
       </c>
       <c r="J8" t="s">
-        <v>165</v>
+        <v>314</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -3551,16 +3707,16 @@
         <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>212</v>
+        <v>171</v>
       </c>
       <c r="H9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I9">
         <v>0.5</v>
       </c>
       <c r="J9" t="s">
-        <v>165</v>
+        <v>314</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -3577,16 +3733,16 @@
         <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>213</v>
+        <v>172</v>
       </c>
       <c r="H10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>165</v>
+        <v>314</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -3603,16 +3759,16 @@
         <v>5</v>
       </c>
       <c r="F11" t="s">
-        <v>221</v>
+        <v>273</v>
       </c>
       <c r="H11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I11">
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>165</v>
+        <v>315</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -3629,97 +3785,97 @@
         <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>222</v>
+        <v>274</v>
       </c>
       <c r="H12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I12">
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>165</v>
+        <v>315</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B13">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C13">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>146</v>
       </c>
       <c r="F13" t="s">
-        <v>223</v>
+        <v>278</v>
       </c>
       <c r="H13" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="I13">
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>165</v>
+        <v>315</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B14">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
       </c>
       <c r="F14" t="s">
-        <v>224</v>
+        <v>275</v>
       </c>
       <c r="H14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I14">
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>165</v>
+        <v>315</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C15">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" t="s">
-        <v>147</v>
+        <v>5</v>
       </c>
       <c r="F15" t="s">
-        <v>218</v>
+        <v>276</v>
       </c>
       <c r="H15" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="I15">
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>165</v>
+        <v>315</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -3736,16 +3892,16 @@
         <v>7</v>
       </c>
       <c r="F16" t="s">
-        <v>219</v>
+        <v>277</v>
       </c>
       <c r="H16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I16">
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>165</v>
+        <v>315</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -3762,16 +3918,16 @@
         <v>7</v>
       </c>
       <c r="F17" t="s">
-        <v>220</v>
+        <v>260</v>
       </c>
       <c r="H17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I17">
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>165</v>
+        <v>315</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -3788,16 +3944,16 @@
         <v>7</v>
       </c>
       <c r="F18" t="s">
-        <v>225</v>
+        <v>261</v>
       </c>
       <c r="H18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I18">
         <v>0.01</v>
       </c>
       <c r="J18" t="s">
-        <v>165</v>
+        <v>315</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -3814,19 +3970,19 @@
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F19" t="s">
-        <v>226</v>
+        <v>262</v>
       </c>
       <c r="H19" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I19">
         <v>0.01</v>
       </c>
       <c r="J19" t="s">
-        <v>165</v>
+        <v>315</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -3843,16 +3999,16 @@
         <v>7</v>
       </c>
       <c r="F20" t="s">
-        <v>214</v>
+        <v>263</v>
       </c>
       <c r="H20" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I20">
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>165</v>
+        <v>255</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -3869,16 +4025,16 @@
         <v>7</v>
       </c>
       <c r="F21" t="s">
-        <v>215</v>
+        <v>264</v>
       </c>
       <c r="H21" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I21">
         <v>0.5</v>
       </c>
       <c r="J21" t="s">
-        <v>165</v>
+        <v>255</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -3895,19 +4051,19 @@
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>216</v>
+        <v>173</v>
       </c>
       <c r="F22" t="s">
-        <v>217</v>
+        <v>265</v>
       </c>
       <c r="H22" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I22">
         <v>0.01</v>
       </c>
       <c r="J22" t="s">
-        <v>165</v>
+        <v>255</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -3924,16 +4080,16 @@
         <v>7</v>
       </c>
       <c r="F23" t="s">
-        <v>227</v>
+        <v>266</v>
       </c>
       <c r="H23" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I23">
         <v>5</v>
       </c>
       <c r="J23" t="s">
-        <v>165</v>
+        <v>255</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -3950,16 +4106,16 @@
         <v>7</v>
       </c>
       <c r="F24" t="s">
-        <v>228</v>
+        <v>266</v>
       </c>
       <c r="H24" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I24">
         <v>5</v>
       </c>
       <c r="J24" t="s">
-        <v>165</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -3972,13 +4128,13 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="33.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4002,24 +4158,24 @@
         <v>144</v>
       </c>
       <c r="G1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" t="s">
         <v>155</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>156</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>157</v>
-      </c>
-      <c r="J1" t="s">
-        <v>158</v>
-      </c>
-      <c r="K1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -4031,19 +4187,19 @@
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I2">
         <v>0.01</v>
       </c>
       <c r="J2" t="s">
-        <v>165</v>
+        <v>313</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -4060,16 +4216,16 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I3">
         <v>1E-3</v>
       </c>
       <c r="J3" t="s">
-        <v>165</v>
+        <v>313</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -4086,16 +4242,16 @@
         <v>7</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="H4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I4">
         <v>1E-3</v>
       </c>
       <c r="J4" t="s">
-        <v>165</v>
+        <v>313</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -4112,16 +4268,16 @@
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>201</v>
+        <v>267</v>
       </c>
       <c r="H5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I5">
         <v>0.01</v>
       </c>
       <c r="J5" t="s">
-        <v>165</v>
+        <v>313</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -4138,16 +4294,16 @@
         <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>202</v>
+        <v>166</v>
       </c>
       <c r="H6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I6">
         <v>0.01</v>
       </c>
       <c r="J6" t="s">
-        <v>165</v>
+        <v>313</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -4164,19 +4320,19 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F7" t="s">
-        <v>203</v>
+        <v>167</v>
       </c>
       <c r="H7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I7">
         <v>0.01</v>
       </c>
       <c r="J7" t="s">
-        <v>165</v>
+        <v>313</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -4193,68 +4349,68 @@
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="H8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I8">
         <v>0.01</v>
       </c>
       <c r="J8" t="s">
-        <v>154</v>
+        <v>315</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>6</v>
+        <v>1.5</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>257</v>
+        <v>269</v>
       </c>
       <c r="H9" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="I9">
         <v>0.01</v>
       </c>
       <c r="J9" t="s">
-        <v>154</v>
+        <v>315</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C10">
-        <v>1.5</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>258</v>
+        <v>272</v>
       </c>
       <c r="H10" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="I10">
         <v>0.01</v>
       </c>
       <c r="J10" t="s">
-        <v>154</v>
+        <v>315</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -4271,16 +4427,16 @@
         <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>259</v>
+        <v>270</v>
       </c>
       <c r="H11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I11">
         <v>0.01</v>
       </c>
       <c r="J11" t="s">
-        <v>154</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -4294,7 +4450,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4323,19 +4479,19 @@
         <v>144</v>
       </c>
       <c r="G1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" t="s">
         <v>155</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>156</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>157</v>
-      </c>
-      <c r="J1" t="s">
-        <v>158</v>
-      </c>
-      <c r="K1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -4352,19 +4508,19 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F2" t="s">
-        <v>169</v>
+        <v>295</v>
       </c>
       <c r="H2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -4381,19 +4537,19 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F3" t="s">
-        <v>170</v>
+        <v>296</v>
       </c>
       <c r="H3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -4410,19 +4566,19 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F4" t="s">
-        <v>171</v>
+        <v>297</v>
       </c>
       <c r="H4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -4439,19 +4595,19 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F5" t="s">
-        <v>182</v>
+        <v>298</v>
       </c>
       <c r="H5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I5">
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -4468,19 +4624,19 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F6" t="s">
-        <v>183</v>
+        <v>299</v>
       </c>
       <c r="H6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I6">
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -4497,19 +4653,19 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F7" t="s">
-        <v>184</v>
+        <v>300</v>
       </c>
       <c r="H7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I7">
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -4526,19 +4682,19 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F8" t="s">
-        <v>185</v>
+        <v>301</v>
       </c>
       <c r="H8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I8">
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -4555,19 +4711,19 @@
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F9" t="s">
-        <v>172</v>
+        <v>302</v>
       </c>
       <c r="H9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -4584,19 +4740,19 @@
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F10" t="s">
-        <v>173</v>
+        <v>287</v>
       </c>
       <c r="H10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -4613,19 +4769,19 @@
         <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F11" t="s">
-        <v>174</v>
+        <v>288</v>
       </c>
       <c r="H11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I11">
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -4642,19 +4798,19 @@
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F12" t="s">
-        <v>175</v>
+        <v>289</v>
       </c>
       <c r="H12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I12">
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -4671,19 +4827,19 @@
         <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F13" t="s">
-        <v>186</v>
+        <v>290</v>
       </c>
       <c r="H13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I13">
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -4700,19 +4856,19 @@
         <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F14" t="s">
-        <v>187</v>
+        <v>291</v>
       </c>
       <c r="H14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I14">
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -4729,19 +4885,19 @@
         <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F15" t="s">
-        <v>188</v>
+        <v>292</v>
       </c>
       <c r="H15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I15">
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -4758,19 +4914,19 @@
         <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F16" t="s">
-        <v>189</v>
+        <v>293</v>
       </c>
       <c r="H16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I16">
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -4787,19 +4943,19 @@
         <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F17" t="s">
-        <v>176</v>
+        <v>294</v>
       </c>
       <c r="H17" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I17">
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -4816,19 +4972,19 @@
         <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F18" t="s">
-        <v>177</v>
+        <v>303</v>
       </c>
       <c r="H18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I18">
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -4845,19 +5001,19 @@
         <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F19" t="s">
-        <v>178</v>
+        <v>304</v>
       </c>
       <c r="H19" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I19">
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -4874,19 +5030,19 @@
         <v>5</v>
       </c>
       <c r="E20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F20" t="s">
-        <v>179</v>
+        <v>305</v>
       </c>
       <c r="H20" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I20">
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -4903,19 +5059,19 @@
         <v>5</v>
       </c>
       <c r="E21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F21" t="s">
-        <v>190</v>
+        <v>306</v>
       </c>
       <c r="H21" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I21">
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -4932,19 +5088,19 @@
         <v>5</v>
       </c>
       <c r="E22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F22" t="s">
-        <v>191</v>
+        <v>307</v>
       </c>
       <c r="H22" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I22">
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -4961,19 +5117,19 @@
         <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F23" t="s">
-        <v>192</v>
+        <v>308</v>
       </c>
       <c r="H23" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I23">
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -4990,19 +5146,19 @@
         <v>5</v>
       </c>
       <c r="E24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F24" t="s">
-        <v>193</v>
+        <v>309</v>
       </c>
       <c r="H24" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I24">
         <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -5019,19 +5175,19 @@
         <v>5</v>
       </c>
       <c r="E25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F25" t="s">
-        <v>180</v>
+        <v>310</v>
       </c>
       <c r="H25" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I25">
         <v>1</v>
       </c>
       <c r="J25" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -5048,19 +5204,19 @@
         <v>5</v>
       </c>
       <c r="E26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F26" t="s">
-        <v>181</v>
+        <v>279</v>
       </c>
       <c r="H26" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I26">
         <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -5077,19 +5233,19 @@
         <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F27" t="s">
-        <v>194</v>
+        <v>280</v>
       </c>
       <c r="H27" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I27">
         <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -5106,19 +5262,19 @@
         <v>5</v>
       </c>
       <c r="E28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F28" t="s">
-        <v>195</v>
+        <v>281</v>
       </c>
       <c r="H28" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I28">
         <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -5135,19 +5291,19 @@
         <v>5</v>
       </c>
       <c r="E29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F29" t="s">
-        <v>196</v>
+        <v>282</v>
       </c>
       <c r="H29" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I29">
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -5164,19 +5320,19 @@
         <v>5</v>
       </c>
       <c r="E30" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F30" t="s">
-        <v>197</v>
+        <v>283</v>
       </c>
       <c r="H30" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I30">
         <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -5193,19 +5349,19 @@
         <v>5</v>
       </c>
       <c r="E31" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F31" t="s">
-        <v>198</v>
+        <v>284</v>
       </c>
       <c r="H31" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I31">
         <v>1</v>
       </c>
       <c r="J31" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
@@ -5222,19 +5378,19 @@
         <v>5</v>
       </c>
       <c r="E32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F32" t="s">
-        <v>199</v>
+        <v>285</v>
       </c>
       <c r="H32" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I32">
         <v>1</v>
       </c>
       <c r="J32" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
@@ -5251,19 +5407,19 @@
         <v>5</v>
       </c>
       <c r="E33" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F33" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="H33" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I33">
         <v>1</v>
       </c>
       <c r="J33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -5277,10 +5433,14 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="55.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -5302,24 +5462,24 @@
         <v>144</v>
       </c>
       <c r="G1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" t="s">
         <v>155</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>156</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>157</v>
-      </c>
-      <c r="J1" t="s">
-        <v>158</v>
-      </c>
-      <c r="K1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>300</v>
+        <v>211</v>
       </c>
       <c r="B2" s="1">
         <v>378</v>
@@ -5331,27 +5491,27 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>204</v>
+        <v>168</v>
       </c>
       <c r="F2" t="s">
-        <v>301</v>
+        <v>212</v>
       </c>
       <c r="G2" t="s">
-        <v>302</v>
+        <v>213</v>
       </c>
       <c r="H2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>303</v>
+        <v>313</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>304</v>
+        <v>214</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -5363,27 +5523,27 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>305</v>
+        <v>215</v>
       </c>
       <c r="F3" t="s">
-        <v>306</v>
+        <v>216</v>
       </c>
       <c r="G3" t="s">
-        <v>307</v>
+        <v>217</v>
       </c>
       <c r="H3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>303</v>
+        <v>313</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>308</v>
+        <v>218</v>
       </c>
       <c r="B4" s="1">
         <v>0.75</v>
@@ -5395,27 +5555,27 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>309</v>
+        <v>219</v>
       </c>
       <c r="F4" t="s">
-        <v>310</v>
+        <v>220</v>
       </c>
       <c r="G4" t="s">
-        <v>311</v>
+        <v>221</v>
       </c>
       <c r="H4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I4">
         <v>1E-3</v>
       </c>
       <c r="J4" t="s">
-        <v>303</v>
+        <v>313</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>312</v>
+        <v>222</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -5427,22 +5587,22 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>204</v>
+        <v>168</v>
       </c>
       <c r="F5" t="s">
+        <v>223</v>
+      </c>
+      <c r="G5" t="s">
+        <v>224</v>
+      </c>
+      <c r="H5" t="s">
+        <v>151</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
         <v>313</v>
-      </c>
-      <c r="G5" t="s">
-        <v>314</v>
-      </c>
-      <c r="H5" t="s">
-        <v>153</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5" t="s">
-        <v>303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>